<commit_message>
fix the item collect drop
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/ItemCollect.xlsx
+++ b/ConfigData/Xlsx/ItemCollect.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -903,7 +903,37 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1151,6 +1181,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4599,20 +4697,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:F87" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:F87" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A3:F87"/>
   <sortState ref="A4:F74">
     <sortCondition ref="A3:A74"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" name="~Name" dataDxfId="4">
+    <tableColumn id="1" name="Id" dataDxfId="8"/>
+    <tableColumn id="2" name="~Name" dataDxfId="7">
       <calculatedColumnFormula>LOOKUP(表2[[#This Row],[Id]],[1]材料!$A:$A,[1]材料!$B:$B)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Type" dataDxfId="3"/>
-    <tableColumn id="25" name="Temperature" dataDxfId="2"/>
-    <tableColumn id="3" name="Humitity" dataDxfId="1"/>
-    <tableColumn id="4" name="Altitude" dataDxfId="0"/>
+    <tableColumn id="16" name="Type" dataDxfId="6"/>
+    <tableColumn id="25" name="Temperature" dataDxfId="5"/>
+    <tableColumn id="3" name="Humitity" dataDxfId="4"/>
+    <tableColumn id="4" name="Altitude" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4626,7 +4724,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -4941,8 +5039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5383,13 +5481,13 @@
         <v>2</v>
       </c>
       <c r="D21" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="6">
         <v>4</v>
       </c>
       <c r="F21" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
@@ -5404,13 +5502,13 @@
         <v>2</v>
       </c>
       <c r="D22" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" s="6">
         <v>2</v>
       </c>
       <c r="F22" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
@@ -5425,7 +5523,7 @@
         <v>2</v>
       </c>
       <c r="D23" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="6">
         <v>3</v>
@@ -5449,7 +5547,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="6">
         <v>2</v>
@@ -5473,7 +5571,7 @@
         <v>2</v>
       </c>
       <c r="F25" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -5512,7 +5610,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="6">
         <v>2</v>
@@ -5530,13 +5628,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F28" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
@@ -5551,13 +5649,13 @@
         <v>2</v>
       </c>
       <c r="D29" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F29" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -5572,13 +5670,13 @@
         <v>2</v>
       </c>
       <c r="D30" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F30" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -5593,13 +5691,13 @@
         <v>2</v>
       </c>
       <c r="D31" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E31" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F31" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -5617,10 +5715,10 @@
         <v>1</v>
       </c>
       <c r="E32" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F32" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
@@ -5635,13 +5733,13 @@
         <v>2</v>
       </c>
       <c r="D33" s="6">
+        <v>2</v>
+      </c>
+      <c r="E33" s="6">
+        <v>3</v>
+      </c>
+      <c r="F33" s="6">
         <v>1</v>
-      </c>
-      <c r="E33" s="6">
-        <v>5</v>
-      </c>
-      <c r="F33" s="6">
-        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
@@ -5656,13 +5754,13 @@
         <v>2</v>
       </c>
       <c r="D34" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E34" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F34" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -5677,13 +5775,13 @@
         <v>2</v>
       </c>
       <c r="D35" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E35" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F35" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
@@ -5701,10 +5799,10 @@
         <v>1</v>
       </c>
       <c r="E36" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F36" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
@@ -5719,13 +5817,13 @@
         <v>2</v>
       </c>
       <c r="D37" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F37" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -5740,13 +5838,13 @@
         <v>2</v>
       </c>
       <c r="D38" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E38" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F38" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -5761,13 +5859,13 @@
         <v>2</v>
       </c>
       <c r="D39" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E39" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F39" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -5782,13 +5880,13 @@
         <v>2</v>
       </c>
       <c r="D40" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F40" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
@@ -5824,13 +5922,13 @@
         <v>3</v>
       </c>
       <c r="D42" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E42" s="6">
         <v>3</v>
       </c>
       <c r="F42" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
@@ -5845,10 +5943,10 @@
         <v>3</v>
       </c>
       <c r="D43" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F43" s="6">
         <v>2</v>
@@ -5866,13 +5964,13 @@
         <v>3</v>
       </c>
       <c r="D44" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
@@ -5887,13 +5985,13 @@
         <v>3</v>
       </c>
       <c r="D45" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E45" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F45" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -5908,13 +6006,13 @@
         <v>3</v>
       </c>
       <c r="D46" s="6">
+        <v>2</v>
+      </c>
+      <c r="E46" s="6">
         <v>4</v>
       </c>
-      <c r="E46" s="6">
-        <v>1</v>
-      </c>
       <c r="F46" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
@@ -5932,10 +6030,10 @@
         <v>2</v>
       </c>
       <c r="E47" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F47" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
@@ -5950,13 +6048,13 @@
         <v>3</v>
       </c>
       <c r="D48" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E48" s="6">
         <v>2</v>
       </c>
       <c r="F48" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
@@ -5971,13 +6069,13 @@
         <v>3</v>
       </c>
       <c r="D49" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E49" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -5998,7 +6096,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
@@ -6013,13 +6111,13 @@
         <v>3</v>
       </c>
       <c r="D51" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E51" s="6">
         <v>2</v>
       </c>
       <c r="F51" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
@@ -6034,7 +6132,7 @@
         <v>3</v>
       </c>
       <c r="D52" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E52" s="6">
         <v>2</v>
@@ -6055,7 +6153,7 @@
         <v>3</v>
       </c>
       <c r="D53" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E53" s="6">
         <v>2</v>
@@ -6076,13 +6174,13 @@
         <v>3</v>
       </c>
       <c r="D54" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E54" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F54" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -6103,7 +6201,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -6118,13 +6216,13 @@
         <v>3</v>
       </c>
       <c r="D56" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F56" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -6139,13 +6237,13 @@
         <v>3</v>
       </c>
       <c r="D57" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E57" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -6160,13 +6258,13 @@
         <v>3</v>
       </c>
       <c r="D58" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E58" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F58" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
@@ -6187,7 +6285,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
@@ -6202,10 +6300,10 @@
         <v>4</v>
       </c>
       <c r="D60" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E60" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F60" s="6">
         <v>2</v>
@@ -6226,10 +6324,10 @@
         <v>4</v>
       </c>
       <c r="E61" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F61" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
@@ -6247,10 +6345,10 @@
         <v>2</v>
       </c>
       <c r="E62" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F62" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
@@ -6268,7 +6366,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F63" s="6">
         <v>1</v>
@@ -6289,10 +6387,10 @@
         <v>2</v>
       </c>
       <c r="E64" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F64" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
@@ -6313,7 +6411,7 @@
         <v>3</v>
       </c>
       <c r="F65" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
@@ -6331,10 +6429,10 @@
         <v>2</v>
       </c>
       <c r="E66" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F66" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
@@ -6352,10 +6450,10 @@
         <v>2</v>
       </c>
       <c r="E67" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F67" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
@@ -6370,13 +6468,13 @@
         <v>4</v>
       </c>
       <c r="D68" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E68" s="6">
         <v>3</v>
       </c>
       <c r="F68" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
@@ -6391,13 +6489,13 @@
         <v>4</v>
       </c>
       <c r="D69" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F69" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
@@ -6412,13 +6510,13 @@
         <v>4</v>
       </c>
       <c r="D70" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E70" s="6">
         <v>3</v>
       </c>
       <c r="F70" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
@@ -6433,13 +6531,13 @@
         <v>5</v>
       </c>
       <c r="D71" s="6">
+        <v>2</v>
+      </c>
+      <c r="E71" s="6">
+        <v>3</v>
+      </c>
+      <c r="F71" s="6">
         <v>1</v>
-      </c>
-      <c r="E71" s="6">
-        <v>1</v>
-      </c>
-      <c r="F71" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
@@ -6475,13 +6573,13 @@
         <v>5</v>
       </c>
       <c r="D73" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E73" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F73" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
@@ -6496,7 +6594,7 @@
         <v>5</v>
       </c>
       <c r="D74" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E74" s="6">
         <v>3</v>
@@ -6517,13 +6615,13 @@
         <v>5</v>
       </c>
       <c r="D75" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E75" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F75" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
@@ -6544,7 +6642,7 @@
         <v>3</v>
       </c>
       <c r="F76" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
@@ -6559,10 +6657,10 @@
         <v>5</v>
       </c>
       <c r="D77" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E77" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F77" s="6">
         <v>2</v>
@@ -6583,7 +6681,7 @@
         <v>2</v>
       </c>
       <c r="E78" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F78" s="6">
         <v>2</v>
@@ -6601,13 +6699,13 @@
         <v>5</v>
       </c>
       <c r="D79" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E79" s="6">
         <v>3</v>
       </c>
       <c r="F79" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
@@ -6628,7 +6726,7 @@
         <v>3</v>
       </c>
       <c r="F80" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
@@ -6643,7 +6741,7 @@
         <v>5</v>
       </c>
       <c r="D81" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E81" s="6">
         <v>3</v>
@@ -6667,10 +6765,10 @@
         <v>2</v>
       </c>
       <c r="E82" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F82" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
@@ -6685,13 +6783,13 @@
         <v>5</v>
       </c>
       <c r="D83" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E83" s="6">
         <v>3</v>
       </c>
       <c r="F83" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
@@ -6706,13 +6804,13 @@
         <v>5</v>
       </c>
       <c r="D84" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E84" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F84" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
@@ -6730,10 +6828,10 @@
         <v>2</v>
       </c>
       <c r="E85" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F85" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
@@ -6748,7 +6846,7 @@
         <v>5</v>
       </c>
       <c r="D86" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E86" s="6">
         <v>3</v>
@@ -6772,37 +6870,52 @@
         <v>2</v>
       </c>
       <c r="E87" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F87" s="6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="D4:F10 D41:F48 D21:F28 D60:F74">
-    <cfRule type="containsBlanks" dxfId="11" priority="30">
+  <conditionalFormatting sqref="D4:F10 D21:F28 D41:F74">
+    <cfRule type="containsBlanks" dxfId="14" priority="33">
       <formula>LEN(TRIM(D4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29:F40">
-    <cfRule type="containsBlanks" dxfId="10" priority="4">
+  <conditionalFormatting sqref="D29:F29 D32:F39">
+    <cfRule type="containsBlanks" dxfId="13" priority="7">
       <formula>LEN(TRIM(D29))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:F56">
-    <cfRule type="containsBlanks" dxfId="9" priority="3">
+    <cfRule type="containsBlanks" dxfId="12" priority="6">
       <formula>LEN(TRIM(D49))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:F59">
-    <cfRule type="containsBlanks" dxfId="8" priority="2">
+    <cfRule type="containsBlanks" dxfId="11" priority="5">
       <formula>LEN(TRIM(D57))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75:F87">
-    <cfRule type="containsBlanks" dxfId="7" priority="1">
+    <cfRule type="containsBlanks" dxfId="10" priority="4">
       <formula>LEN(TRIM(D75))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:F30">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(D30))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31:F39">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(D31))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:F40">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(D40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>